<commit_message>
update reading usecase function
</commit_message>
<xml_diff>
--- a/project/resources/annotations.xlsx
+++ b/project/resources/annotations.xlsx
@@ -1,23 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\file-project\project\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2080DD23-CA2D-45F6-A33B-86A2EF33B2BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E721EAD-D23B-425B-9267-86CB65EE0347}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{8CC964DB-4A15-4676-8746-8279EF0C1367}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4" xr2:uid="{8CC964DB-4A15-4676-8746-8279EF0C1367}"/>
   </bookViews>
   <sheets>
     <sheet name="elements" sheetId="1" r:id="rId1"/>
     <sheet name="states" sheetId="2" r:id="rId2"/>
     <sheet name="flows" sheetId="3" r:id="rId3"/>
     <sheet name="events" sheetId="4" r:id="rId4"/>
-    <sheet name="annotations" sheetId="5" r:id="rId5"/>
+    <sheet name="event_list" sheetId="6" r:id="rId5"/>
+    <sheet name="annotations" sheetId="5" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="67">
   <si>
     <t>text input</t>
   </si>
@@ -215,6 +216,33 @@
   </si>
   <si>
     <t>100.</t>
+  </si>
+  <si>
+    <t>list of events</t>
+  </si>
+  <si>
+    <t>^\{(?:\d+)'*\.(\s)+(?:\d+)'*\.}</t>
+  </si>
+  <si>
+    <t>{1. 2.}</t>
+  </si>
+  <si>
+    <t>{5'. 12.}</t>
+  </si>
+  <si>
+    <t>{8'. 15}</t>
+  </si>
+  <si>
+    <t>^\[(?:\d+)'*\.(\s)+(?:\d+)'*\.\,([0-9A-Za-z\s])+]</t>
+  </si>
+  <si>
+    <t>[5'.  12., flow b]</t>
+  </si>
+  <si>
+    <t>[1. 2., flow a]</t>
+  </si>
+  <si>
+    <t>[8'.  15., flow c]</t>
   </si>
 </sst>
 </file>
@@ -282,7 +310,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -320,11 +348,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="5" tint="0.59999389629810485"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -363,8 +400,17 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1001,10 +1047,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9B004DF-7224-4B85-BFF3-28DE6EBD813C}">
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1017,17 +1063,17 @@
       <c r="A1" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="16" t="s">
+      <c r="B1" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>27</v>
@@ -1036,18 +1082,18 @@
         <v>28</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>55</v>
+        <v>29</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>56</v>
+        <v>30</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>57</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B3" s="6" t="s">
         <v>27</v>
@@ -1056,18 +1102,18 @@
         <v>28</v>
       </c>
       <c r="D3" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="F3" s="6" t="s">
         <v>29</v>
-      </c>
-      <c r="E3" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="F3" s="6" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
-        <v>43</v>
+        <v>54</v>
       </c>
       <c r="B4" s="6" t="s">
         <v>27</v>
@@ -1076,13 +1122,13 @@
         <v>28</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>32</v>
+        <v>55</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>33</v>
+        <v>56</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>29</v>
+        <v>57</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
@@ -1108,14 +1154,6 @@
       <c r="D7" s="7"/>
       <c r="E7" s="7"/>
       <c r="F7" s="7"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A8" s="5"/>
-      <c r="B8" s="5"/>
-      <c r="C8" s="7"/>
-      <c r="D8" s="7"/>
-      <c r="E8" s="7"/>
-      <c r="F8" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1127,6 +1165,66 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0601B3A5-53E0-4422-B75A-9BE9D6697625}">
+  <dimension ref="A1:D3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="76" customWidth="1"/>
+    <col min="2" max="4" width="33.5546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="B1" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="16" t="s">
+        <v>63</v>
+      </c>
+      <c r="B2" s="16" t="s">
+        <v>65</v>
+      </c>
+      <c r="C2" s="16" t="s">
+        <v>64</v>
+      </c>
+      <c r="D2" s="16" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="16" t="s">
+        <v>59</v>
+      </c>
+      <c r="B3" s="16" t="s">
+        <v>60</v>
+      </c>
+      <c r="C3" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="D3" s="16" t="s">
+        <v>62</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B1:D1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9A64D41-9CBE-4E65-B308-62DC0E12F075}">
   <dimension ref="A1:F15"/>
   <sheetViews>
@@ -1144,13 +1242,13 @@
       <c r="A1" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="17" t="s">
+      <c r="B1" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
-      <c r="F1" s="17"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">

</xml_diff>